<commit_message>
Die Commandbars Einstellungen (cbar.enable = false bzw cbar.enable = true) rausgenommen; diese Veränderungen haben nur unangenehme Seiteneffekte auf Std Excel und werden eigentlich gar nicht benötigt. Es reicht völlig, den Rechts Click in der Projekt Tafel in der Event Routine zu disablen: cancel = true
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/Projectboard.xlsx
+++ b/Projectboard/Projectboard/Projectboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="2415" windowWidth="22695" windowHeight="8325" activeTab="1"/>
+    <workbookView xWindow="345" yWindow="1500" windowWidth="24765" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -354,11 +354,13 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -367,7 +369,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -395,6 +397,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
.EnableEvents in den Name und Hierarchie-Formularen auf false gesetzt, wenn es sich denn um ShowDialog Formular Aufrufe handelt. Das muss gemacht werden, um den Excel Event Trigger auszuschalten der z.B. kommt wenn von Excel zu Powerpoint und wieder zurück gewechselt wird ... Das fürher t dann zu Fehlern in der Activate(.panes) Routine.
EnableEvents in den okButton Click Routinen dann nicht einfach auf true gesetzt, sondern auf den Wert, den es vorher hatte (false oder true) . Das wird über den Konstrukt formerEE gemacht, der den EingangsWert von appinstance.EnableEvents aufnimmt
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/Projectboard.xlsx
+++ b/Projectboard/Projectboard/Projectboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2790" windowWidth="9270" windowHeight="7230"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="10875" windowHeight="7980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -354,7 +354,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
@@ -369,7 +371,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Schreibschutz für Projectboard.xlsx aktiviert, damit es von mehreren gleichzeitig von einem Remote Directory gestartet werden kann awinGeneralModules ergänzt / korrigiert: - Import des Projectboard XML Konfi Files
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/Projectboard.xlsx
+++ b/Projectboard/Projectboard/Projectboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2790" windowWidth="11805" windowHeight="5085" activeTab="1"/>
+    <workbookView xWindow="1560" yWindow="3060" windowWidth="8790" windowHeight="5160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -395,9 +395,14 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+  </cols>
   <sheetData/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Vorbereitung für modify Attributes, modify Termine ..
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/Projectboard.xlsx
+++ b/Projectboard/Projectboard/Projectboard.xlsx
@@ -4,12 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="3060" windowWidth="8790" windowHeight="5160" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="2130" windowWidth="12240" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
+    <sheet name="Tabelle5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -371,7 +373,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -395,7 +397,7 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
@@ -408,4 +410,30 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle4"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle5"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
enableOnUpdate für MassenEdit auf Off gesetzt; meistens ohne Probleme Massen-Edit mit zwei Windows ...
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/Projectboard.xlsx
+++ b/Projectboard/Projectboard/Projectboard.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="2130" windowWidth="12240" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="16650" windowHeight="12300" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
-    <sheet name="Tabelle4" sheetId="4" r:id="rId4"/>
-    <sheet name="Tabelle5" sheetId="5" r:id="rId5"/>
+    <sheet name="MPT" sheetId="1" r:id="rId1"/>
+    <sheet name="meRC" sheetId="2" r:id="rId2"/>
+    <sheet name="meTE" sheetId="3" r:id="rId3"/>
+    <sheet name="meAT" sheetId="4" r:id="rId4"/>
+    <sheet name="meCharts" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -373,7 +373,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -421,7 +421,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -430,10 +432,12 @@
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Windows V0.9 zur Darstellung von Portfolio und Projekt Charts
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/Projectboard.xlsx
+++ b/Projectboard/Projectboard/Projectboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1260" windowWidth="16650" windowHeight="12300" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="930" windowWidth="14670" windowHeight="12630"/>
   </bookViews>
   <sheets>
     <sheet name="MPT" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,8 @@
     <sheet name="meTE" sheetId="3" r:id="rId3"/>
     <sheet name="meAT" sheetId="4" r:id="rId4"/>
     <sheet name="meCharts" sheetId="5" r:id="rId5"/>
+    <sheet name="mptPrCharts" sheetId="6" r:id="rId6"/>
+    <sheet name="mptPfCharts" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -356,7 +358,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -432,7 +434,35 @@
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle6"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle7"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>

<commit_message>
edit Termine v0.7 Hierarchie getnextIDofId : Fehler korrigiert ..
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/Projectboard.xlsx
+++ b/Projectboard/Projectboard/Projectboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="2130" windowWidth="7725" windowHeight="12300" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="4890" yWindow="2130" windowWidth="20220" windowHeight="8580" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MPT" sheetId="1" r:id="rId1"/>
@@ -50,10 +50,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,14 +403,41 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="1" max="1" width="10.25" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="3" max="3" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="18.375" customWidth="1"/>
+    <col min="5" max="6" width="12.625" customWidth="1"/>
+    <col min="7" max="7" width="5" customWidth="1"/>
+    <col min="8" max="9" width="35.625" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="7.25" customWidth="1"/>
   </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle4"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -415,9 +445,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Tabelle4"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -430,9 +460,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Tabelle5"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle6"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -445,9 +488,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Tabelle6"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle8"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -456,32 +499,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Tabelle7"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Tabelle8"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>